<commit_message>
Menú lateral. Actualización Fase 2 (Jhorman)
</commit_message>
<xml_diff>
--- a/DiagramaGantt.xlsx
+++ b/DiagramaGantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8eae290e31edaf6/Horario_EKIRIA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5E7C2C50-3690-41BA-913F-D3AE4B526E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12FAFE2-80F5-44ED-9E76-DFA7FDFD59DD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2A693A1-0B2B-44E8-B0E3-0FC50624FE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="19440" windowHeight="10590" xr2:uid="{81CC7B3D-AB92-4DD1-893B-26F9E8267843}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{81CC7B3D-AB92-4DD1-893B-26F9E8267843}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>ekiria</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Reunión cliente</t>
+  </si>
+  <si>
+    <t>Creación del menú lateral de usuario(Prediseño)</t>
   </si>
 </sst>
 </file>
@@ -422,36 +425,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +441,36 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,12 +887,12 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="33" width="3.7109375" customWidth="1"/>
@@ -900,18 +903,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:37" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="17">
@@ -921,62 +924,62 @@
         <f>D5+D4</f>
         <v>44470</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="27">
         <f>G5</f>
         <v>44470</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="19">
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="27">
         <f>N5</f>
         <v>44477</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="19">
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="27">
         <f>U5</f>
         <v>44484</v>
       </c>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="26">
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="34">
         <f>AB5</f>
         <v>44491</v>
       </c>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="19">
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="27">
         <f>AI5</f>
         <v>44498</v>
       </c>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="21"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="29"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="32">
         <v>44470</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="6"/>
       <c r="G5" s="3">
         <f>E4</f>
@@ -1246,13 +1249,13 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1287,7 +1290,7 @@
       <c r="AK7" s="7"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1296,10 +1299,10 @@
       <c r="C8" s="9">
         <v>0</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="23">
         <v>44480</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="23">
         <v>44482</v>
       </c>
       <c r="F8" s="7"/>
@@ -1336,7 +1339,7 @@
       <c r="AK8" s="7"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1345,10 +1348,10 @@
       <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="24">
         <v>44483</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="24">
         <v>44490</v>
       </c>
       <c r="F9" s="7"/>
@@ -1385,7 +1388,7 @@
       <c r="AK9" s="7"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1394,10 +1397,10 @@
       <c r="C10" s="9">
         <v>0.25</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="24">
         <v>44487</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="24">
         <v>44491</v>
       </c>
       <c r="F10" s="7"/>
@@ -1434,7 +1437,7 @@
       <c r="AK10" s="7"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1443,10 +1446,10 @@
       <c r="C11" s="9">
         <v>0</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="24">
         <v>44487</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="24">
         <v>44491</v>
       </c>
       <c r="F11" s="7"/>
@@ -1483,7 +1486,7 @@
       <c r="AK11" s="7"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1492,10 +1495,10 @@
       <c r="C12" s="9">
         <v>0</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="23">
         <v>44493</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="23">
         <v>44493</v>
       </c>
       <c r="F12" s="7"/>
@@ -1532,13 +1535,13 @@
       <c r="AK12" s="7"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -1573,11 +1576,21 @@
       <c r="AK13" s="7"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>44498</v>
+      </c>
+      <c r="E14" s="10">
+        <v>44499</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>

</xml_diff>

<commit_message>
Actualización. Termine el menú lateral de usuario
</commit_message>
<xml_diff>
--- a/DiagramaGantt.xlsx
+++ b/DiagramaGantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Horario_EKIRIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2A693A1-0B2B-44E8-B0E3-0FC50624FE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35990808-BC21-4C91-BD34-52ADE61E546C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{81CC7B3D-AB92-4DD1-893B-26F9E8267843}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ekiria</t>
   </si>
@@ -887,7 +887,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1583,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="10">
         <v>44498</v>
@@ -1627,11 +1627,21 @@
       <c r="AK14" s="7"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="A15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="10">
+        <v>44501</v>
+      </c>
+      <c r="E15" s="10">
+        <v>44522</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>

</xml_diff>